<commit_message>
task: add Concentration column in template.
import concentration and update sample

feat: Add concentration column to wellplate list

fix: test coverage for purity value

fixed failing tests for spreadsheet, lint

fixed lint error
</commit_message>
<xml_diff>
--- a/spec/fixtures/import/wellplate_import_template.xlsx
+++ b/spec/fixtures/import/wellplate_import_template.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhaubold/projects/KIT/chemotion_ELN/public/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\zaib\complat\chemotion_ELN\spec\fixtures\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D234F10B-06D8-3548-995D-F9EE33E56EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1208246-245F-47E4-8C73-DFF5E76FD24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wellplate import template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="107">
   <si>
     <t>Position</t>
   </si>
@@ -338,6 +343,9 @@
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>Concentration</t>
   </si>
 </sst>
 </file>
@@ -1675,27 +1683,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1708,1936 +1717,2035 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="15">
+      <c r="E2" s="7"/>
+      <c r="F2" s="15">
         <v>0.1</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="13">
+      <c r="E3" s="11"/>
+      <c r="F3" s="13">
         <v>0.2</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="12">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="13">
+      <c r="E4" s="11"/>
+      <c r="F4" s="13">
         <v>0.3</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="12">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="13">
+      <c r="E5" s="11"/>
+      <c r="F5" s="13">
         <v>0.4</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="12">
         <v>4</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="13">
+      <c r="E6" s="11"/>
+      <c r="F6" s="13">
         <v>0.5</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="12">
         <v>5</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="13">
+      <c r="E7" s="11"/>
+      <c r="F7" s="13">
         <v>0.6</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="12">
         <v>6</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="13">
+      <c r="E8" s="11"/>
+      <c r="F8" s="13">
         <v>0.7</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="12">
         <v>7</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="13">
+      <c r="E9" s="11"/>
+      <c r="F9" s="13">
         <v>0.8</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="G9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="11">
         <v>8</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="13">
+      <c r="E10" s="11"/>
+      <c r="F10" s="13">
         <v>0.9</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="G10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="11">
         <v>9</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="13">
+      <c r="E11" s="11"/>
+      <c r="F11" s="13">
         <v>0.1</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="11">
+      <c r="G11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="11">
         <v>10</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="13">
+      <c r="E12" s="11"/>
+      <c r="F12" s="13">
         <v>0.11</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="G12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="11">
         <v>11</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="13">
+      <c r="E13" s="11"/>
+      <c r="F13" s="13">
         <v>0.12</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="G13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="11">
         <v>12</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="13">
+      <c r="E14" s="11"/>
+      <c r="F14" s="13">
         <v>0.13</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="11">
+      <c r="G14" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="11">
         <v>13</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="13">
+      <c r="E15" s="11"/>
+      <c r="F15" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="G15" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="11">
         <v>14</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="13">
+      <c r="E16" s="11"/>
+      <c r="F16" s="13">
         <v>0.15</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="G16" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="11">
         <v>15</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="13">
+      <c r="E17" s="11"/>
+      <c r="F17" s="13">
         <v>0.16</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="G17" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="11">
         <v>16</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="16">
+      <c r="E18" s="11"/>
+      <c r="F18" s="16">
         <v>0.17</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="G18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="12">
         <v>17</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="16">
+      <c r="E19" s="11"/>
+      <c r="F19" s="16">
         <v>0.18</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="12">
         <v>18</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="16">
+      <c r="E20" s="11"/>
+      <c r="F20" s="16">
         <v>0.19</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G20" s="12">
+      <c r="G20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="12">
         <v>19</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="13">
+      <c r="E21" s="11"/>
+      <c r="F21" s="13">
         <v>0.2</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="11">
+      <c r="G21" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="11">
         <v>20</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="13">
+      <c r="E22" s="11"/>
+      <c r="F22" s="13">
         <v>0.21</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" s="12">
+      <c r="G22" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="12">
         <v>21</v>
       </c>
-      <c r="H22" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
-      <c r="E23" s="13">
+      <c r="E23" s="11"/>
+      <c r="F23" s="13">
         <v>0.22</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="11">
+      <c r="G23" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="11">
         <v>22</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="13">
+      <c r="E24" s="11"/>
+      <c r="F24" s="13">
         <v>0.23</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" s="12">
+      <c r="G24" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="12">
         <v>23</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="13">
+      <c r="E25" s="11"/>
+      <c r="F25" s="13">
         <v>0.24</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="11">
+      <c r="G25" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="11">
         <v>24</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="13">
+      <c r="E26" s="11"/>
+      <c r="F26" s="13">
         <v>0.25</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="11">
+      <c r="G26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="11">
         <v>25</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
-      <c r="E27" s="13">
+      <c r="E27" s="11"/>
+      <c r="F27" s="13">
         <v>0.26</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G27" s="12">
+      <c r="G27" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="12">
         <v>26</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="13">
+      <c r="E28" s="11"/>
+      <c r="F28" s="13">
         <v>0.27</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G28" s="12">
+      <c r="G28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="12">
         <v>27</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="13">
+      <c r="E29" s="11"/>
+      <c r="F29" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G29" s="12">
+      <c r="G29" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="12">
         <v>28</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="13">
+      <c r="E30" s="11"/>
+      <c r="F30" s="13">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="12">
+      <c r="G30" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="12">
         <v>29</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="13">
+      <c r="E31" s="11"/>
+      <c r="F31" s="13">
         <v>0.3</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G31" s="12">
+      <c r="G31" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="12">
         <v>30</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I31" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="13">
+      <c r="E32" s="11"/>
+      <c r="F32" s="13">
         <v>0.31</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G32" s="12">
+      <c r="G32" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="12">
         <v>31</v>
       </c>
-      <c r="H32" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I32" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="13">
+      <c r="E33" s="11"/>
+      <c r="F33" s="13">
         <v>0.32</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="12">
+      <c r="G33" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="12">
         <v>32</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I33" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="13">
+      <c r="E34" s="11"/>
+      <c r="F34" s="13">
         <v>0.33</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="11">
+      <c r="G34" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="11">
         <v>33</v>
       </c>
-      <c r="H34" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I34" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="13">
+      <c r="E35" s="11"/>
+      <c r="F35" s="13">
         <v>0.34</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G35" s="11">
+      <c r="G35" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="11">
         <v>34</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I35" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="13">
+      <c r="E36" s="11"/>
+      <c r="F36" s="13">
         <v>0.35</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" s="11">
+      <c r="G36" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="11">
         <v>35</v>
       </c>
-      <c r="H36" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I36" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
-      <c r="E37" s="13">
+      <c r="E37" s="11"/>
+      <c r="F37" s="13">
         <v>0.36</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G37" s="11">
+      <c r="G37" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" s="11">
         <v>36</v>
       </c>
-      <c r="H37" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I37" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
-      <c r="E38" s="13">
+      <c r="E38" s="11"/>
+      <c r="F38" s="13">
         <v>0.37</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G38" s="11">
+      <c r="G38" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="11">
         <v>37</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I38" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="13">
+      <c r="E39" s="11"/>
+      <c r="F39" s="13">
         <v>0.38</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G39" s="11">
+      <c r="G39" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="11">
         <v>38</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I39" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
-      <c r="E40" s="13">
+      <c r="E40" s="11"/>
+      <c r="F40" s="13">
         <v>0.39</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G40" s="11">
+      <c r="G40" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="11">
         <v>39</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I40" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
-      <c r="E41" s="13">
+      <c r="E41" s="11"/>
+      <c r="F41" s="13">
         <v>0.4</v>
       </c>
-      <c r="F41" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G41" s="11">
+      <c r="G41" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="11">
         <v>40</v>
       </c>
-      <c r="H41" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I41" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
-      <c r="E42" s="13">
+      <c r="E42" s="11"/>
+      <c r="F42" s="13">
         <v>0.41</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="11">
+      <c r="G42" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H42" s="11">
         <v>41</v>
       </c>
-      <c r="H42" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I42" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
-      <c r="E43" s="13">
+      <c r="E43" s="11"/>
+      <c r="F43" s="13">
         <v>0.42</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="12">
+      <c r="G43" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" s="12">
         <v>42</v>
       </c>
-      <c r="H43" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I43" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
-      <c r="E44" s="13">
+      <c r="E44" s="11"/>
+      <c r="F44" s="13">
         <v>0.43</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" s="12">
+      <c r="G44" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H44" s="12">
         <v>43</v>
       </c>
-      <c r="H44" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I44" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
-      <c r="E45" s="13">
+      <c r="E45" s="11"/>
+      <c r="F45" s="13">
         <v>0.44</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G45" s="12">
+      <c r="G45" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H45" s="12">
         <v>44</v>
       </c>
-      <c r="H45" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I45" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="13">
+      <c r="E46" s="11"/>
+      <c r="F46" s="13">
         <v>0.45</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G46" s="11">
+      <c r="G46" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="11">
         <v>45</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I46" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
-      <c r="E47" s="13">
+      <c r="E47" s="11"/>
+      <c r="F47" s="13">
         <v>0.46</v>
       </c>
-      <c r="F47" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47" s="12">
+      <c r="G47" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="12">
         <v>46</v>
       </c>
-      <c r="H47" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I47" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
-      <c r="E48" s="13">
+      <c r="E48" s="11"/>
+      <c r="F48" s="13">
         <v>0.47</v>
       </c>
-      <c r="F48" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48" s="11">
+      <c r="G48" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H48" s="11">
         <v>47</v>
       </c>
-      <c r="H48" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I48" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="13">
+      <c r="E49" s="11"/>
+      <c r="F49" s="13">
         <v>0.48</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" s="12">
+      <c r="G49" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="12">
         <v>48</v>
       </c>
-      <c r="H49" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I49" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="13">
+      <c r="E50" s="11"/>
+      <c r="F50" s="13">
         <v>0.49</v>
       </c>
-      <c r="F50" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G50" s="11">
+      <c r="G50" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="11">
         <v>49</v>
       </c>
-      <c r="H50" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I50" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
-      <c r="E51" s="13">
+      <c r="E51" s="11"/>
+      <c r="F51" s="13">
         <v>0.5</v>
       </c>
-      <c r="F51" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G51" s="11">
+      <c r="G51" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="11">
         <v>50</v>
       </c>
-      <c r="H51" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I51" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
-      <c r="E52" s="13">
+      <c r="E52" s="11"/>
+      <c r="F52" s="13">
         <v>0.51</v>
       </c>
-      <c r="F52" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" s="11">
+      <c r="G52" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" s="11">
         <v>51</v>
       </c>
-      <c r="H52" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I52" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
-      <c r="E53" s="13">
+      <c r="E53" s="11"/>
+      <c r="F53" s="13">
         <v>0.52</v>
       </c>
-      <c r="F53" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53" s="11">
+      <c r="G53" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="11">
         <v>52</v>
       </c>
-      <c r="H53" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I53" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
-      <c r="E54" s="13">
+      <c r="E54" s="11"/>
+      <c r="F54" s="13">
         <v>0.53</v>
       </c>
-      <c r="F54" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G54" s="11">
+      <c r="G54" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H54" s="11">
         <v>53</v>
       </c>
-      <c r="H54" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I54" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
-      <c r="E55" s="13">
+      <c r="E55" s="11"/>
+      <c r="F55" s="13">
         <v>0.54</v>
       </c>
-      <c r="F55" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G55" s="11">
+      <c r="G55" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" s="11">
         <v>54</v>
       </c>
-      <c r="H55" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I55" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
-      <c r="E56" s="13">
+      <c r="E56" s="11"/>
+      <c r="F56" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F56" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G56" s="11">
+      <c r="G56" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="11">
         <v>55</v>
       </c>
-      <c r="H56" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I56" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
-      <c r="E57" s="13">
+      <c r="E57" s="11"/>
+      <c r="F57" s="13">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F57" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G57" s="11">
+      <c r="G57" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H57" s="11">
         <v>56</v>
       </c>
-      <c r="H57" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I57" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
-      <c r="E58" s="13">
+      <c r="E58" s="11"/>
+      <c r="F58" s="13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F58" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G58" s="11">
+      <c r="G58" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H58" s="11">
         <v>57</v>
       </c>
-      <c r="H58" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I58" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
-      <c r="E59" s="13">
+      <c r="E59" s="11"/>
+      <c r="F59" s="13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F59" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G59" s="11">
+      <c r="G59" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" s="11">
         <v>58</v>
       </c>
-      <c r="H59" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I59" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>63</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
-      <c r="E60" s="13">
+      <c r="E60" s="11"/>
+      <c r="F60" s="13">
         <v>0.59</v>
       </c>
-      <c r="F60" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G60" s="11">
+      <c r="G60" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H60" s="11">
         <v>59</v>
       </c>
-      <c r="H60" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I60" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
-      <c r="E61" s="13">
+      <c r="E61" s="11"/>
+      <c r="F61" s="13">
         <v>0.6</v>
       </c>
-      <c r="F61" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G61" s="11">
+      <c r="G61" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" s="11">
         <v>60</v>
       </c>
-      <c r="H61" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I61" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
-      <c r="E62" s="13">
+      <c r="E62" s="11"/>
+      <c r="F62" s="13">
         <v>0.61</v>
       </c>
-      <c r="F62" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G62" s="11">
+      <c r="G62" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H62" s="11">
         <v>61</v>
       </c>
-      <c r="H62" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I62" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
-      <c r="E63" s="13">
+      <c r="E63" s="11"/>
+      <c r="F63" s="13">
         <v>0.62</v>
       </c>
-      <c r="F63" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G63" s="11">
+      <c r="G63" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H63" s="11">
         <v>62</v>
       </c>
-      <c r="H63" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I63" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
-      <c r="E64" s="13">
+      <c r="E64" s="11"/>
+      <c r="F64" s="13">
         <v>0.63</v>
       </c>
-      <c r="F64" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G64" s="11">
+      <c r="G64" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H64" s="11">
         <v>63</v>
       </c>
-      <c r="H64" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I64" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
-      <c r="E65" s="13">
+      <c r="E65" s="11"/>
+      <c r="F65" s="13">
         <v>0.64</v>
       </c>
-      <c r="F65" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G65" s="11">
+      <c r="G65" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H65" s="11">
         <v>64</v>
       </c>
-      <c r="H65" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I65" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
-      <c r="E66" s="13">
+      <c r="E66" s="11"/>
+      <c r="F66" s="13">
         <v>0.65</v>
       </c>
-      <c r="F66" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G66" s="11">
+      <c r="G66" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H66" s="11">
         <v>65</v>
       </c>
-      <c r="H66" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I66" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="13">
+      <c r="E67" s="11"/>
+      <c r="F67" s="13">
         <v>0.66</v>
       </c>
-      <c r="F67" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G67" s="11">
+      <c r="G67" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H67" s="11">
         <v>66</v>
       </c>
-      <c r="H67" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I67" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="13">
+      <c r="E68" s="11"/>
+      <c r="F68" s="13">
         <v>0.67</v>
       </c>
-      <c r="F68" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G68" s="11">
+      <c r="G68" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H68" s="11">
         <v>67</v>
       </c>
-      <c r="H68" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I68" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="13">
+      <c r="E69" s="11"/>
+      <c r="F69" s="13">
         <v>0.68</v>
       </c>
-      <c r="F69" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G69" s="11">
+      <c r="G69" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H69" s="11">
         <v>68</v>
       </c>
-      <c r="H69" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I69" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>73</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="13">
+      <c r="E70" s="11"/>
+      <c r="F70" s="13">
         <v>0.69</v>
       </c>
-      <c r="F70" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G70" s="11">
+      <c r="G70" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H70" s="11">
         <v>69</v>
       </c>
-      <c r="H70" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I70" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="13">
+      <c r="E71" s="11"/>
+      <c r="F71" s="13">
         <v>0.7</v>
       </c>
-      <c r="F71" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G71" s="11">
+      <c r="G71" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H71" s="11">
         <v>70</v>
       </c>
-      <c r="H71" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I71" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="13">
+      <c r="E72" s="11"/>
+      <c r="F72" s="13">
         <v>0.71</v>
       </c>
-      <c r="F72" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G72" s="11">
+      <c r="G72" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H72" s="11">
         <v>71</v>
       </c>
-      <c r="H72" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I72" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
-      <c r="E73" s="13">
+      <c r="E73" s="11"/>
+      <c r="F73" s="13">
         <v>0.72</v>
       </c>
-      <c r="F73" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G73" s="11">
+      <c r="G73" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H73" s="11">
         <v>72</v>
       </c>
-      <c r="H73" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I73" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
-      <c r="E74" s="13">
+      <c r="E74" s="11"/>
+      <c r="F74" s="13">
         <v>0.73</v>
       </c>
-      <c r="F74" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G74" s="11">
+      <c r="G74" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H74" s="11">
         <v>73</v>
       </c>
-      <c r="H74" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I74" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
-      <c r="E75" s="13">
+      <c r="E75" s="11"/>
+      <c r="F75" s="13">
         <v>0.74</v>
       </c>
-      <c r="F75" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G75" s="11">
+      <c r="G75" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H75" s="11">
         <v>74</v>
       </c>
-      <c r="H75" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I75" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
-      <c r="E76" s="13">
+      <c r="E76" s="11"/>
+      <c r="F76" s="13">
         <v>0.75</v>
       </c>
-      <c r="F76" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G76" s="11">
+      <c r="G76" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H76" s="11">
         <v>75</v>
       </c>
-      <c r="H76" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I76" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
-      <c r="E77" s="13">
+      <c r="E77" s="11"/>
+      <c r="F77" s="13">
         <v>0.76</v>
       </c>
-      <c r="F77" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G77" s="11">
+      <c r="G77" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H77" s="11">
         <v>76</v>
       </c>
-      <c r="H77" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I77" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
-      <c r="E78" s="13">
+      <c r="E78" s="11"/>
+      <c r="F78" s="13">
         <v>0.77</v>
       </c>
-      <c r="F78" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G78" s="11">
+      <c r="G78" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H78" s="11">
         <v>77</v>
       </c>
-      <c r="H78" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I78" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>82</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
-      <c r="E79" s="13">
+      <c r="E79" s="11"/>
+      <c r="F79" s="13">
         <v>0.78</v>
       </c>
-      <c r="F79" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G79" s="11">
+      <c r="G79" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H79" s="11">
         <v>78</v>
       </c>
-      <c r="H79" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I79" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
-      <c r="E80" s="13">
+      <c r="E80" s="11"/>
+      <c r="F80" s="13">
         <v>0.79</v>
       </c>
-      <c r="F80" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G80" s="11">
+      <c r="G80" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H80" s="11">
         <v>79</v>
       </c>
-      <c r="H80" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I80" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
-      <c r="E81" s="13">
+      <c r="E81" s="11"/>
+      <c r="F81" s="13">
         <v>0.8</v>
       </c>
-      <c r="F81" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G81" s="11">
+      <c r="G81" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H81" s="11">
         <v>80</v>
       </c>
-      <c r="H81" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I81" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
-      <c r="E82" s="13">
+      <c r="E82" s="11"/>
+      <c r="F82" s="13">
         <v>0.81</v>
       </c>
-      <c r="F82" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G82" s="11">
+      <c r="G82" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H82" s="11">
         <v>81</v>
       </c>
-      <c r="H82" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I82" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
-      <c r="E83" s="13">
+      <c r="E83" s="11"/>
+      <c r="F83" s="13">
         <v>0.82</v>
       </c>
-      <c r="F83" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G83" s="11">
+      <c r="G83" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H83" s="11">
         <v>82</v>
       </c>
-      <c r="H83" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I83" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
-      <c r="E84" s="13">
+      <c r="E84" s="11"/>
+      <c r="F84" s="13">
         <v>0.83</v>
       </c>
-      <c r="F84" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G84" s="11">
+      <c r="G84" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H84" s="11">
         <v>83</v>
       </c>
-      <c r="H84" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I84" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
-      <c r="E85" s="13">
+      <c r="E85" s="11"/>
+      <c r="F85" s="13">
         <v>0.84</v>
       </c>
-      <c r="F85" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G85" s="11">
+      <c r="G85" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H85" s="11">
         <v>84</v>
       </c>
-      <c r="H85" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I85" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
-      <c r="E86" s="13">
+      <c r="E86" s="11"/>
+      <c r="F86" s="13">
         <v>0.85</v>
       </c>
-      <c r="F86" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G86" s="11">
+      <c r="G86" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H86" s="11">
         <v>85</v>
       </c>
-      <c r="H86" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I86" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
-      <c r="E87" s="13">
+      <c r="E87" s="11"/>
+      <c r="F87" s="13">
         <v>0.86</v>
       </c>
-      <c r="F87" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G87" s="11">
+      <c r="G87" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H87" s="11">
         <v>86</v>
       </c>
-      <c r="H87" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I87" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
-      <c r="E88" s="13">
+      <c r="E88" s="11"/>
+      <c r="F88" s="13">
         <v>0.87</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G88" s="11">
+      <c r="G88" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H88" s="11">
         <v>87</v>
       </c>
-      <c r="H88" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I88" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
-      <c r="E89" s="13">
+      <c r="E89" s="11"/>
+      <c r="F89" s="13">
         <v>0.88</v>
       </c>
-      <c r="F89" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G89" s="11">
+      <c r="G89" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H89" s="11">
         <v>88</v>
       </c>
-      <c r="H89" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I89" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
-      <c r="E90" s="13">
+      <c r="E90" s="11"/>
+      <c r="F90" s="13">
         <v>0.89</v>
       </c>
-      <c r="F90" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G90" s="11">
+      <c r="G90" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H90" s="11">
         <v>89</v>
       </c>
-      <c r="H90" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I90" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>94</v>
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
-      <c r="E91" s="13">
+      <c r="E91" s="11"/>
+      <c r="F91" s="13">
         <v>0.9</v>
       </c>
-      <c r="F91" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G91" s="11">
+      <c r="G91" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H91" s="11">
         <v>90</v>
       </c>
-      <c r="H91" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I91" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>95</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
-      <c r="E92" s="13">
+      <c r="E92" s="11"/>
+      <c r="F92" s="13">
         <v>0.91</v>
       </c>
-      <c r="F92" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G92" s="11">
+      <c r="G92" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H92" s="11">
         <v>91</v>
       </c>
-      <c r="H92" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I92" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
-      <c r="E93" s="13">
+      <c r="E93" s="11"/>
+      <c r="F93" s="13">
         <v>0.92</v>
       </c>
-      <c r="F93" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G93" s="11">
+      <c r="G93" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H93" s="11">
         <v>92</v>
       </c>
-      <c r="H93" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I93" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>97</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
-      <c r="E94" s="13">
+      <c r="E94" s="11"/>
+      <c r="F94" s="13">
         <v>0.93</v>
       </c>
-      <c r="F94" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G94" s="11">
+      <c r="G94" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H94" s="11">
         <v>93</v>
       </c>
-      <c r="H94" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I94" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
-      <c r="E95" s="13">
+      <c r="E95" s="11"/>
+      <c r="F95" s="13">
         <v>0.94</v>
       </c>
-      <c r="F95" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G95" s="11">
+      <c r="G95" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H95" s="11">
         <v>94</v>
       </c>
-      <c r="H95" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I95" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
-      <c r="E96" s="13">
+      <c r="E96" s="11"/>
+      <c r="F96" s="13">
         <v>0.95</v>
       </c>
-      <c r="F96" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G96" s="11">
+      <c r="G96" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H96" s="11">
         <v>95</v>
       </c>
-      <c r="H96" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I96" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
-      <c r="E97" s="13">
+      <c r="E97" s="11"/>
+      <c r="F97" s="13">
         <v>0.96</v>
       </c>
-      <c r="F97" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G97" s="11">
+      <c r="G97" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H97" s="11">
         <v>96</v>
       </c>
-      <c r="H97" s="11" t="s">
+      <c r="I97" s="11" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: changed concentration to Molarity on wellplate update.
fix: failing test for template creation

ui: show Molarity unit next to input

import header
</commit_message>
<xml_diff>
--- a/spec/fixtures/import/wellplate_import_template.xlsx
+++ b/spec/fixtures/import/wellplate_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\zaib\complat\chemotion_ELN\spec\fixtures\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1208246-245F-47E4-8C73-DFF5E76FD24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD291AC-2910-471E-B239-CC0947EF0119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33855" yWindow="2130" windowWidth="28800" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wellplate import template" sheetId="1" r:id="rId1"/>
@@ -345,7 +345,7 @@
     <t>Sample</t>
   </si>
   <si>
-    <t>Concentration</t>
+    <t>Molarity (M)</t>
   </si>
 </sst>
 </file>
@@ -1685,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="M85" sqref="M85"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: update sample molarity in wellplate (#2848)
</commit_message>
<xml_diff>
--- a/spec/fixtures/import/wellplate_import_template.xlsx
+++ b/spec/fixtures/import/wellplate_import_template.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhaubold/projects/KIT/chemotion_ELN/public/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\zaib\complat\chemotion_ELN\spec\fixtures\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D234F10B-06D8-3548-995D-F9EE33E56EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD291AC-2910-471E-B239-CC0947EF0119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33855" yWindow="2130" windowWidth="28800" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wellplate import template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="107">
   <si>
     <t>Position</t>
   </si>
@@ -338,6 +343,9 @@
   </si>
   <si>
     <t>Sample</t>
+  </si>
+  <si>
+    <t>Molarity (M)</t>
   </si>
 </sst>
 </file>
@@ -1675,27 +1683,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="28" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="20.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1708,1936 +1717,2035 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="15">
+      <c r="E2" s="7"/>
+      <c r="F2" s="15">
         <v>0.1</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="13">
+      <c r="E3" s="11"/>
+      <c r="F3" s="13">
         <v>0.2</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="12">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="13">
+      <c r="E4" s="11"/>
+      <c r="F4" s="13">
         <v>0.3</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="12">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="13">
+      <c r="E5" s="11"/>
+      <c r="F5" s="13">
         <v>0.4</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="12">
+      <c r="G5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="12">
         <v>4</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="13">
+      <c r="E6" s="11"/>
+      <c r="F6" s="13">
         <v>0.5</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="G6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H6" s="12">
         <v>5</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="13">
+      <c r="E7" s="11"/>
+      <c r="F7" s="13">
         <v>0.6</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G7" s="12">
+      <c r="G7" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="12">
         <v>6</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="13">
+      <c r="E8" s="11"/>
+      <c r="F8" s="13">
         <v>0.7</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="G8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="12">
         <v>7</v>
       </c>
-      <c r="H8" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-      <c r="E9" s="13">
+      <c r="E9" s="11"/>
+      <c r="F9" s="13">
         <v>0.8</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="G9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="11">
         <v>8</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="13">
+      <c r="E10" s="11"/>
+      <c r="F10" s="13">
         <v>0.9</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="G10" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="11">
         <v>9</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="13">
+      <c r="E11" s="11"/>
+      <c r="F11" s="13">
         <v>0.1</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="11">
+      <c r="G11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="11">
         <v>10</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="13">
+      <c r="E12" s="11"/>
+      <c r="F12" s="13">
         <v>0.11</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="G12" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="11">
         <v>11</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="13">
+      <c r="E13" s="11"/>
+      <c r="F13" s="13">
         <v>0.12</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="G13" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="11">
         <v>12</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="13">
+      <c r="E14" s="11"/>
+      <c r="F14" s="13">
         <v>0.13</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G14" s="11">
+      <c r="G14" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="11">
         <v>13</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="13">
+      <c r="E15" s="11"/>
+      <c r="F15" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="G15" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="11">
         <v>14</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="13">
+      <c r="E16" s="11"/>
+      <c r="F16" s="13">
         <v>0.15</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="G16" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="11">
         <v>15</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="13">
+      <c r="E17" s="11"/>
+      <c r="F17" s="13">
         <v>0.16</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="G17" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="11">
         <v>16</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
-      <c r="E18" s="16">
+      <c r="E18" s="11"/>
+      <c r="F18" s="16">
         <v>0.17</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="G18" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="12">
         <v>17</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
-      <c r="E19" s="16">
+      <c r="E19" s="11"/>
+      <c r="F19" s="16">
         <v>0.18</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="12">
         <v>18</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="16">
+      <c r="E20" s="11"/>
+      <c r="F20" s="16">
         <v>0.19</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G20" s="12">
+      <c r="G20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H20" s="12">
         <v>19</v>
       </c>
-      <c r="H20" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="13">
+      <c r="E21" s="11"/>
+      <c r="F21" s="13">
         <v>0.2</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="11">
+      <c r="G21" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H21" s="11">
         <v>20</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-      <c r="E22" s="13">
+      <c r="E22" s="11"/>
+      <c r="F22" s="13">
         <v>0.21</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" s="12">
+      <c r="G22" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="12">
         <v>21</v>
       </c>
-      <c r="H22" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
-      <c r="E23" s="13">
+      <c r="E23" s="11"/>
+      <c r="F23" s="13">
         <v>0.22</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="11">
+      <c r="G23" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="11">
         <v>22</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="13">
+      <c r="E24" s="11"/>
+      <c r="F24" s="13">
         <v>0.23</v>
       </c>
-      <c r="F24" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" s="12">
+      <c r="G24" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="12">
         <v>23</v>
       </c>
-      <c r="H24" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="13">
+      <c r="E25" s="11"/>
+      <c r="F25" s="13">
         <v>0.24</v>
       </c>
-      <c r="F25" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="11">
+      <c r="G25" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="11">
         <v>24</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="13">
+      <c r="E26" s="11"/>
+      <c r="F26" s="13">
         <v>0.25</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G26" s="11">
+      <c r="G26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="11">
         <v>25</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
-      <c r="E27" s="13">
+      <c r="E27" s="11"/>
+      <c r="F27" s="13">
         <v>0.26</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G27" s="12">
+      <c r="G27" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="12">
         <v>26</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="13">
+      <c r="E28" s="11"/>
+      <c r="F28" s="13">
         <v>0.27</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G28" s="12">
+      <c r="G28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="12">
         <v>27</v>
       </c>
-      <c r="H28" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="13">
+      <c r="E29" s="11"/>
+      <c r="F29" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G29" s="12">
+      <c r="G29" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="12">
         <v>28</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="13">
+      <c r="E30" s="11"/>
+      <c r="F30" s="13">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="12">
+      <c r="G30" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="12">
         <v>29</v>
       </c>
-      <c r="H30" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="13">
+      <c r="E31" s="11"/>
+      <c r="F31" s="13">
         <v>0.3</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G31" s="12">
+      <c r="G31" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="12">
         <v>30</v>
       </c>
-      <c r="H31" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I31" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="13">
+      <c r="E32" s="11"/>
+      <c r="F32" s="13">
         <v>0.31</v>
       </c>
-      <c r="F32" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G32" s="12">
+      <c r="G32" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="12">
         <v>31</v>
       </c>
-      <c r="H32" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I32" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="13">
+      <c r="E33" s="11"/>
+      <c r="F33" s="13">
         <v>0.32</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="12">
+      <c r="G33" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="12">
         <v>32</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I33" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="13">
+      <c r="E34" s="11"/>
+      <c r="F34" s="13">
         <v>0.33</v>
       </c>
-      <c r="F34" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="11">
+      <c r="G34" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="11">
         <v>33</v>
       </c>
-      <c r="H34" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I34" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="13">
+      <c r="E35" s="11"/>
+      <c r="F35" s="13">
         <v>0.34</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G35" s="11">
+      <c r="G35" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H35" s="11">
         <v>34</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I35" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="13">
+      <c r="E36" s="11"/>
+      <c r="F36" s="13">
         <v>0.35</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" s="11">
+      <c r="G36" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="11">
         <v>35</v>
       </c>
-      <c r="H36" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I36" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
-      <c r="E37" s="13">
+      <c r="E37" s="11"/>
+      <c r="F37" s="13">
         <v>0.36</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G37" s="11">
+      <c r="G37" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" s="11">
         <v>36</v>
       </c>
-      <c r="H37" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I37" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
-      <c r="E38" s="13">
+      <c r="E38" s="11"/>
+      <c r="F38" s="13">
         <v>0.37</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G38" s="11">
+      <c r="G38" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="11">
         <v>37</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I38" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="13">
+      <c r="E39" s="11"/>
+      <c r="F39" s="13">
         <v>0.38</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G39" s="11">
+      <c r="G39" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="11">
         <v>38</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I39" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
-      <c r="E40" s="13">
+      <c r="E40" s="11"/>
+      <c r="F40" s="13">
         <v>0.39</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G40" s="11">
+      <c r="G40" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="11">
         <v>39</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I40" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
-      <c r="E41" s="13">
+      <c r="E41" s="11"/>
+      <c r="F41" s="13">
         <v>0.4</v>
       </c>
-      <c r="F41" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G41" s="11">
+      <c r="G41" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="11">
         <v>40</v>
       </c>
-      <c r="H41" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I41" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
-      <c r="E42" s="13">
+      <c r="E42" s="11"/>
+      <c r="F42" s="13">
         <v>0.41</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="11">
+      <c r="G42" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H42" s="11">
         <v>41</v>
       </c>
-      <c r="H42" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I42" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
-      <c r="E43" s="13">
+      <c r="E43" s="11"/>
+      <c r="F43" s="13">
         <v>0.42</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="12">
+      <c r="G43" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" s="12">
         <v>42</v>
       </c>
-      <c r="H43" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I43" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
-      <c r="E44" s="13">
+      <c r="E44" s="11"/>
+      <c r="F44" s="13">
         <v>0.43</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G44" s="12">
+      <c r="G44" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H44" s="12">
         <v>43</v>
       </c>
-      <c r="H44" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I44" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
-      <c r="E45" s="13">
+      <c r="E45" s="11"/>
+      <c r="F45" s="13">
         <v>0.44</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G45" s="12">
+      <c r="G45" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H45" s="12">
         <v>44</v>
       </c>
-      <c r="H45" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I45" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="13">
+      <c r="E46" s="11"/>
+      <c r="F46" s="13">
         <v>0.45</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G46" s="11">
+      <c r="G46" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="11">
         <v>45</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I46" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
-      <c r="E47" s="13">
+      <c r="E47" s="11"/>
+      <c r="F47" s="13">
         <v>0.46</v>
       </c>
-      <c r="F47" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G47" s="12">
+      <c r="G47" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="12">
         <v>46</v>
       </c>
-      <c r="H47" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I47" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
-      <c r="E48" s="13">
+      <c r="E48" s="11"/>
+      <c r="F48" s="13">
         <v>0.47</v>
       </c>
-      <c r="F48" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G48" s="11">
+      <c r="G48" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H48" s="11">
         <v>47</v>
       </c>
-      <c r="H48" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I48" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="13">
+      <c r="E49" s="11"/>
+      <c r="F49" s="13">
         <v>0.48</v>
       </c>
-      <c r="F49" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G49" s="12">
+      <c r="G49" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="12">
         <v>48</v>
       </c>
-      <c r="H49" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I49" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="13">
+      <c r="E50" s="11"/>
+      <c r="F50" s="13">
         <v>0.49</v>
       </c>
-      <c r="F50" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G50" s="11">
+      <c r="G50" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="11">
         <v>49</v>
       </c>
-      <c r="H50" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I50" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
-      <c r="E51" s="13">
+      <c r="E51" s="11"/>
+      <c r="F51" s="13">
         <v>0.5</v>
       </c>
-      <c r="F51" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G51" s="11">
+      <c r="G51" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="11">
         <v>50</v>
       </c>
-      <c r="H51" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I51" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
-      <c r="E52" s="13">
+      <c r="E52" s="11"/>
+      <c r="F52" s="13">
         <v>0.51</v>
       </c>
-      <c r="F52" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" s="11">
+      <c r="G52" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" s="11">
         <v>51</v>
       </c>
-      <c r="H52" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I52" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
-      <c r="E53" s="13">
+      <c r="E53" s="11"/>
+      <c r="F53" s="13">
         <v>0.52</v>
       </c>
-      <c r="F53" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53" s="11">
+      <c r="G53" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" s="11">
         <v>52</v>
       </c>
-      <c r="H53" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I53" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
-      <c r="E54" s="13">
+      <c r="E54" s="11"/>
+      <c r="F54" s="13">
         <v>0.53</v>
       </c>
-      <c r="F54" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G54" s="11">
+      <c r="G54" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H54" s="11">
         <v>53</v>
       </c>
-      <c r="H54" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I54" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
-      <c r="E55" s="13">
+      <c r="E55" s="11"/>
+      <c r="F55" s="13">
         <v>0.54</v>
       </c>
-      <c r="F55" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G55" s="11">
+      <c r="G55" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" s="11">
         <v>54</v>
       </c>
-      <c r="H55" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I55" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
-      <c r="E56" s="13">
+      <c r="E56" s="11"/>
+      <c r="F56" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F56" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G56" s="11">
+      <c r="G56" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H56" s="11">
         <v>55</v>
       </c>
-      <c r="H56" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I56" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
-      <c r="E57" s="13">
+      <c r="E57" s="11"/>
+      <c r="F57" s="13">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F57" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G57" s="11">
+      <c r="G57" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H57" s="11">
         <v>56</v>
       </c>
-      <c r="H57" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I57" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
-      <c r="E58" s="13">
+      <c r="E58" s="11"/>
+      <c r="F58" s="13">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F58" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G58" s="11">
+      <c r="G58" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H58" s="11">
         <v>57</v>
       </c>
-      <c r="H58" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I58" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
-      <c r="E59" s="13">
+      <c r="E59" s="11"/>
+      <c r="F59" s="13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F59" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G59" s="11">
+      <c r="G59" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" s="11">
         <v>58</v>
       </c>
-      <c r="H59" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I59" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>63</v>
       </c>
       <c r="B60" s="10"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
-      <c r="E60" s="13">
+      <c r="E60" s="11"/>
+      <c r="F60" s="13">
         <v>0.59</v>
       </c>
-      <c r="F60" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G60" s="11">
+      <c r="G60" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H60" s="11">
         <v>59</v>
       </c>
-      <c r="H60" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I60" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
-      <c r="E61" s="13">
+      <c r="E61" s="11"/>
+      <c r="F61" s="13">
         <v>0.6</v>
       </c>
-      <c r="F61" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G61" s="11">
+      <c r="G61" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" s="11">
         <v>60</v>
       </c>
-      <c r="H61" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I61" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
-      <c r="E62" s="13">
+      <c r="E62" s="11"/>
+      <c r="F62" s="13">
         <v>0.61</v>
       </c>
-      <c r="F62" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G62" s="11">
+      <c r="G62" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H62" s="11">
         <v>61</v>
       </c>
-      <c r="H62" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I62" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
-      <c r="E63" s="13">
+      <c r="E63" s="11"/>
+      <c r="F63" s="13">
         <v>0.62</v>
       </c>
-      <c r="F63" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G63" s="11">
+      <c r="G63" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H63" s="11">
         <v>62</v>
       </c>
-      <c r="H63" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I63" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="10"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
-      <c r="E64" s="13">
+      <c r="E64" s="11"/>
+      <c r="F64" s="13">
         <v>0.63</v>
       </c>
-      <c r="F64" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G64" s="11">
+      <c r="G64" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H64" s="11">
         <v>63</v>
       </c>
-      <c r="H64" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I64" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>68</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
-      <c r="E65" s="13">
+      <c r="E65" s="11"/>
+      <c r="F65" s="13">
         <v>0.64</v>
       </c>
-      <c r="F65" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G65" s="11">
+      <c r="G65" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H65" s="11">
         <v>64</v>
       </c>
-      <c r="H65" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I65" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
-      <c r="E66" s="13">
+      <c r="E66" s="11"/>
+      <c r="F66" s="13">
         <v>0.65</v>
       </c>
-      <c r="F66" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G66" s="11">
+      <c r="G66" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H66" s="11">
         <v>65</v>
       </c>
-      <c r="H66" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I66" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="13">
+      <c r="E67" s="11"/>
+      <c r="F67" s="13">
         <v>0.66</v>
       </c>
-      <c r="F67" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G67" s="11">
+      <c r="G67" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H67" s="11">
         <v>66</v>
       </c>
-      <c r="H67" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I67" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>71</v>
       </c>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="13">
+      <c r="E68" s="11"/>
+      <c r="F68" s="13">
         <v>0.67</v>
       </c>
-      <c r="F68" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G68" s="11">
+      <c r="G68" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H68" s="11">
         <v>67</v>
       </c>
-      <c r="H68" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I68" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="13">
+      <c r="E69" s="11"/>
+      <c r="F69" s="13">
         <v>0.68</v>
       </c>
-      <c r="F69" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G69" s="11">
+      <c r="G69" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H69" s="11">
         <v>68</v>
       </c>
-      <c r="H69" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I69" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>73</v>
       </c>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="13">
+      <c r="E70" s="11"/>
+      <c r="F70" s="13">
         <v>0.69</v>
       </c>
-      <c r="F70" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G70" s="11">
+      <c r="G70" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H70" s="11">
         <v>69</v>
       </c>
-      <c r="H70" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I70" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="13">
+      <c r="E71" s="11"/>
+      <c r="F71" s="13">
         <v>0.7</v>
       </c>
-      <c r="F71" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G71" s="11">
+      <c r="G71" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H71" s="11">
         <v>70</v>
       </c>
-      <c r="H71" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I71" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>75</v>
       </c>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="13">
+      <c r="E72" s="11"/>
+      <c r="F72" s="13">
         <v>0.71</v>
       </c>
-      <c r="F72" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G72" s="11">
+      <c r="G72" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H72" s="11">
         <v>71</v>
       </c>
-      <c r="H72" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I72" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>76</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
-      <c r="E73" s="13">
+      <c r="E73" s="11"/>
+      <c r="F73" s="13">
         <v>0.72</v>
       </c>
-      <c r="F73" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G73" s="11">
+      <c r="G73" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H73" s="11">
         <v>72</v>
       </c>
-      <c r="H73" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I73" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
-      <c r="E74" s="13">
+      <c r="E74" s="11"/>
+      <c r="F74" s="13">
         <v>0.73</v>
       </c>
-      <c r="F74" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G74" s="11">
+      <c r="G74" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H74" s="11">
         <v>73</v>
       </c>
-      <c r="H74" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I74" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>78</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
-      <c r="E75" s="13">
+      <c r="E75" s="11"/>
+      <c r="F75" s="13">
         <v>0.74</v>
       </c>
-      <c r="F75" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G75" s="11">
+      <c r="G75" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H75" s="11">
         <v>74</v>
       </c>
-      <c r="H75" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I75" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
-      <c r="E76" s="13">
+      <c r="E76" s="11"/>
+      <c r="F76" s="13">
         <v>0.75</v>
       </c>
-      <c r="F76" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G76" s="11">
+      <c r="G76" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H76" s="11">
         <v>75</v>
       </c>
-      <c r="H76" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I76" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>80</v>
       </c>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
-      <c r="E77" s="13">
+      <c r="E77" s="11"/>
+      <c r="F77" s="13">
         <v>0.76</v>
       </c>
-      <c r="F77" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G77" s="11">
+      <c r="G77" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H77" s="11">
         <v>76</v>
       </c>
-      <c r="H77" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I77" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
-      <c r="E78" s="13">
+      <c r="E78" s="11"/>
+      <c r="F78" s="13">
         <v>0.77</v>
       </c>
-      <c r="F78" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G78" s="11">
+      <c r="G78" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H78" s="11">
         <v>77</v>
       </c>
-      <c r="H78" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I78" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>82</v>
       </c>
       <c r="B79" s="10"/>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
-      <c r="E79" s="13">
+      <c r="E79" s="11"/>
+      <c r="F79" s="13">
         <v>0.78</v>
       </c>
-      <c r="F79" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G79" s="11">
+      <c r="G79" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H79" s="11">
         <v>78</v>
       </c>
-      <c r="H79" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I79" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="10"/>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
-      <c r="E80" s="13">
+      <c r="E80" s="11"/>
+      <c r="F80" s="13">
         <v>0.79</v>
       </c>
-      <c r="F80" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G80" s="11">
+      <c r="G80" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H80" s="11">
         <v>79</v>
       </c>
-      <c r="H80" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I80" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B81" s="10"/>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
-      <c r="E81" s="13">
+      <c r="E81" s="11"/>
+      <c r="F81" s="13">
         <v>0.8</v>
       </c>
-      <c r="F81" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G81" s="11">
+      <c r="G81" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H81" s="11">
         <v>80</v>
       </c>
-      <c r="H81" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I81" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="10"/>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
-      <c r="E82" s="13">
+      <c r="E82" s="11"/>
+      <c r="F82" s="13">
         <v>0.81</v>
       </c>
-      <c r="F82" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G82" s="11">
+      <c r="G82" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H82" s="11">
         <v>81</v>
       </c>
-      <c r="H82" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I82" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
-      <c r="E83" s="13">
+      <c r="E83" s="11"/>
+      <c r="F83" s="13">
         <v>0.82</v>
       </c>
-      <c r="F83" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G83" s="11">
+      <c r="G83" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H83" s="11">
         <v>82</v>
       </c>
-      <c r="H83" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I83" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
-      <c r="E84" s="13">
+      <c r="E84" s="11"/>
+      <c r="F84" s="13">
         <v>0.83</v>
       </c>
-      <c r="F84" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G84" s="11">
+      <c r="G84" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H84" s="11">
         <v>83</v>
       </c>
-      <c r="H84" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I84" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
-      <c r="E85" s="13">
+      <c r="E85" s="11"/>
+      <c r="F85" s="13">
         <v>0.84</v>
       </c>
-      <c r="F85" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G85" s="11">
+      <c r="G85" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H85" s="11">
         <v>84</v>
       </c>
-      <c r="H85" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I85" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="10"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
-      <c r="E86" s="13">
+      <c r="E86" s="11"/>
+      <c r="F86" s="13">
         <v>0.85</v>
       </c>
-      <c r="F86" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G86" s="11">
+      <c r="G86" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H86" s="11">
         <v>85</v>
       </c>
-      <c r="H86" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I86" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="10"/>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
-      <c r="E87" s="13">
+      <c r="E87" s="11"/>
+      <c r="F87" s="13">
         <v>0.86</v>
       </c>
-      <c r="F87" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G87" s="11">
+      <c r="G87" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H87" s="11">
         <v>86</v>
       </c>
-      <c r="H87" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I87" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="10"/>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
-      <c r="E88" s="13">
+      <c r="E88" s="11"/>
+      <c r="F88" s="13">
         <v>0.87</v>
       </c>
-      <c r="F88" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G88" s="11">
+      <c r="G88" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H88" s="11">
         <v>87</v>
       </c>
-      <c r="H88" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I88" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
-      <c r="E89" s="13">
+      <c r="E89" s="11"/>
+      <c r="F89" s="13">
         <v>0.88</v>
       </c>
-      <c r="F89" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G89" s="11">
+      <c r="G89" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H89" s="11">
         <v>88</v>
       </c>
-      <c r="H89" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I89" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
-      <c r="E90" s="13">
+      <c r="E90" s="11"/>
+      <c r="F90" s="13">
         <v>0.89</v>
       </c>
-      <c r="F90" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G90" s="11">
+      <c r="G90" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H90" s="11">
         <v>89</v>
       </c>
-      <c r="H90" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I90" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>94</v>
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
-      <c r="E91" s="13">
+      <c r="E91" s="11"/>
+      <c r="F91" s="13">
         <v>0.9</v>
       </c>
-      <c r="F91" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G91" s="11">
+      <c r="G91" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H91" s="11">
         <v>90</v>
       </c>
-      <c r="H91" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I91" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>95</v>
       </c>
       <c r="B92" s="10"/>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
-      <c r="E92" s="13">
+      <c r="E92" s="11"/>
+      <c r="F92" s="13">
         <v>0.91</v>
       </c>
-      <c r="F92" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G92" s="11">
+      <c r="G92" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H92" s="11">
         <v>91</v>
       </c>
-      <c r="H92" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I92" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>96</v>
       </c>
       <c r="B93" s="10"/>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
-      <c r="E93" s="13">
+      <c r="E93" s="11"/>
+      <c r="F93" s="13">
         <v>0.92</v>
       </c>
-      <c r="F93" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G93" s="11">
+      <c r="G93" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H93" s="11">
         <v>92</v>
       </c>
-      <c r="H93" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I93" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>97</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
-      <c r="E94" s="13">
+      <c r="E94" s="11"/>
+      <c r="F94" s="13">
         <v>0.93</v>
       </c>
-      <c r="F94" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G94" s="11">
+      <c r="G94" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H94" s="11">
         <v>93</v>
       </c>
-      <c r="H94" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I94" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B95" s="10"/>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
-      <c r="E95" s="13">
+      <c r="E95" s="11"/>
+      <c r="F95" s="13">
         <v>0.94</v>
       </c>
-      <c r="F95" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G95" s="11">
+      <c r="G95" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H95" s="11">
         <v>94</v>
       </c>
-      <c r="H95" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I95" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="10"/>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
-      <c r="E96" s="13">
+      <c r="E96" s="11"/>
+      <c r="F96" s="13">
         <v>0.95</v>
       </c>
-      <c r="F96" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G96" s="11">
+      <c r="G96" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H96" s="11">
         <v>95</v>
       </c>
-      <c r="H96" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I96" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>100</v>
       </c>
       <c r="B97" s="10"/>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
-      <c r="E97" s="13">
+      <c r="E97" s="11"/>
+      <c r="F97" s="13">
         <v>0.96</v>
       </c>
-      <c r="F97" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G97" s="11">
+      <c r="G97" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H97" s="11">
         <v>96</v>
       </c>
-      <c r="H97" s="11" t="s">
+      <c r="I97" s="11" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>